<commit_message>
changes to v6 spreadsheet template
</commit_message>
<xml_diff>
--- a/Documents/IndoPacific/indoPacificTemplate_v6.xlsx
+++ b/Documents/IndoPacific/indoPacificTemplate_v6.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37120" windowHeight="16680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="14280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -14,10 +14,10 @@
   <definedNames>
     <definedName name="basisOfID">Lists!$B$2:$B$3</definedName>
     <definedName name="biome">Lists!$D$2:$D$26</definedName>
-    <definedName name="georeferenceProtocol" localSheetId="0">Instructions!$C$28</definedName>
+    <definedName name="georeferenceProtocol" localSheetId="0">Instructions!$C$29</definedName>
     <definedName name="habitat">Lists!$E$2:$E$13</definedName>
-    <definedName name="maximumDistanceAboveSurfaceInMeters" localSheetId="0">Instructions!$C$22</definedName>
-    <definedName name="minimumDistanceAboveSurfaceInMeters" localSheetId="0">Instructions!$C$20</definedName>
+    <definedName name="maximumDistanceAboveSurfaceInMeters" localSheetId="0">Instructions!$C$23</definedName>
+    <definedName name="minimumDistanceAboveSurfaceInMeters" localSheetId="0">Instructions!$C$21</definedName>
     <definedName name="ownerInstitute">Lists!$C$2:$C$12</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -631,7 +631,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="319">
   <si>
     <t>materialSampleID</t>
   </si>
@@ -1242,9 +1242,6 @@
     <t>substrate from which the individual was sampled</t>
   </si>
   <si>
-    <t>Please pick from the list</t>
-  </si>
-  <si>
     <t>in meters</t>
   </si>
   <si>
@@ -1332,9 +1329,6 @@
     <t>maximumDistanceAboveSurfaceInMeters</t>
   </si>
   <si>
-    <t>define a list?</t>
-  </si>
-  <si>
     <t>validation (must be positive, must be less than max as abs val)</t>
   </si>
   <si>
@@ -1410,18 +1404,12 @@
     <t>referring to the length of the organism from which the sample was derived</t>
   </si>
   <si>
-    <t>well</t>
-  </si>
-  <si>
     <t>plateId</t>
   </si>
   <si>
     <t>tissueStorageId</t>
   </si>
   <si>
-    <t>Identifier for the plate that tissue was put in</t>
-  </si>
-  <si>
     <t>previousTissueId</t>
   </si>
   <si>
@@ -1512,9 +1500,6 @@
     <t>Full Name (A list (concatenated and separated) of names of people, groups, or organizations who assigned the Taxon to the subject.)</t>
   </si>
   <si>
-    <t>Sequence-Specific Data, provided when uploading sequence formats only</t>
-  </si>
-  <si>
     <t>probably doesn't need to go here</t>
   </si>
   <si>
@@ -1524,15 +1509,9 @@
     <t>sequencingFacility</t>
   </si>
   <si>
-    <t>The facility that sequenced this e.g. MVZ, UQ, UCLA [THE INSTITUTION THAT GENERATED THE GENETIC DATA]</t>
-  </si>
-  <si>
     <t>Person who generated this data.</t>
   </si>
   <si>
-    <t>personWhoGeneratedData</t>
-  </si>
-  <si>
     <t>Mat. Sample</t>
   </si>
   <si>
@@ -1540,6 +1519,75 @@
   </si>
   <si>
     <t>warning if not there; required OR locality</t>
+  </si>
+  <si>
+    <t>Please pick from the list - see lists tab.</t>
+  </si>
+  <si>
+    <t>choose from list (must use one of the values else its an error unless its null)</t>
+  </si>
+  <si>
+    <t>microHabitat</t>
+  </si>
+  <si>
+    <t>More specific habitat field</t>
+  </si>
+  <si>
+    <t>choose from list of microhabitats but can also write new ones not in the list</t>
+  </si>
+  <si>
+    <t>extractionId</t>
+  </si>
+  <si>
+    <t>Genotypic-Specific Data, provided when uploading genotypic formats only</t>
+  </si>
+  <si>
+    <t>wellId</t>
+  </si>
+  <si>
+    <t>A platename where the DNA extract is stored</t>
+  </si>
+  <si>
+    <t>The well on the plate where the DNA extract is stored</t>
+  </si>
+  <si>
+    <t>A unique identifier for the extraction (other than plate or well)</t>
+  </si>
+  <si>
+    <t>An identiifier for the container which holds the material sample</t>
+  </si>
+  <si>
+    <t>individualID</t>
+  </si>
+  <si>
+    <t>A unique identifier for a particular individual</t>
+  </si>
+  <si>
+    <t>http://rs.tdwg.org/dwc/terms/individualID</t>
+  </si>
+  <si>
+    <t>equal to the MaterialSampleId if this is left blank.</t>
+  </si>
+  <si>
+    <t>personWhoGeneratedGeneticData</t>
+  </si>
+  <si>
+    <t>The facility that generated the genetic data</t>
+  </si>
+  <si>
+    <t>scoringMethod</t>
+  </si>
+  <si>
+    <t>e.g. computer-binned, manual/user allele calls, migration distance</t>
+  </si>
+  <si>
+    <t>genotypingMethod</t>
+  </si>
+  <si>
+    <t>e.g. capillary electrophoresis, gel electrophoresis, illumina, 454, ion torrent, micro-array, qpcr, solid</t>
+  </si>
+  <si>
+    <t>use a list</t>
   </si>
 </sst>
 </file>
@@ -1549,7 +1597,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1658,6 +1706,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1771,7 +1824,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="84">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1856,8 +1909,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2002,8 +2058,9 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="84">
+  <cellStyles count="87">
     <cellStyle name="Bad" xfId="65" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -2054,6 +2111,9 @@
     <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2416,15 +2476,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="41" customWidth="1"/>
+    <col min="1" max="1" width="25" style="41" customWidth="1"/>
     <col min="2" max="2" width="41.1640625" style="41" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="18.83203125" style="41" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" style="41" customWidth="1"/>
@@ -2445,10 +2505,10 @@
         <v>125</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E1" s="23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F1" s="23" t="s">
         <v>199</v>
@@ -2462,7 +2522,7 @@
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="29" thickTop="1">
       <c r="A2" s="48" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>129</v>
@@ -2471,16 +2531,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>130</v>
       </c>
       <c r="G2" s="49" t="str">
-        <f t="shared" ref="G2:G74" si="0">CONCATENATE("&lt;attribute column='",$C2,"' uri='",$F2,"' /&gt;")</f>
+        <f t="shared" ref="G2:G77" si="0">CONCATENATE("&lt;attribute column='",$C2,"' uri='",$F2,"' /&gt;")</f>
         <v>&lt;attribute column='materialSampleID' uri='http://rs.tdwg.org/dwc/terms/MaterialSampleID' /&gt;</v>
       </c>
       <c r="H2" s="50" t="s">
@@ -2507,7 +2567,7 @@
         <v>&lt;attribute column='enteredBy' uri='urn:enteredBy' /&gt;</v>
       </c>
       <c r="H3" s="26" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -2530,7 +2590,7 @@
         <v>&lt;attribute column='yearEntered' uri='urn:yearEntered' /&gt;</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -2553,7 +2613,7 @@
         <v>&lt;attribute column='monthEntered' uri='urn:monthEntered' /&gt;</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2576,7 +2636,7 @@
         <v>&lt;attribute column='dayEntered' uri='urn:dayEntered' /&gt;</v>
       </c>
       <c r="H6" s="26" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2585,25 +2645,25 @@
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="26" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="12" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
@@ -2612,7 +2672,7 @@
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="6" customFormat="1">
@@ -2623,18 +2683,18 @@
         <v>129</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G9" s="48"/>
       <c r="H9" s="50" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2648,7 +2708,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
@@ -2671,7 +2731,7 @@
         <v>8</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
@@ -2694,7 +2754,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="s">
@@ -2717,7 +2777,7 @@
         <v>10</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13" t="s">
@@ -2743,7 +2803,7 @@
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>146</v>
@@ -2753,7 +2813,7 @@
         <v>&lt;attribute column='biome' uri='http://purl.obolibrary.org/obo/ENVO_00000428' /&gt;</v>
       </c>
       <c r="H14" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2768,7 +2828,7 @@
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13" t="s">
-        <v>233</v>
+        <v>297</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>147</v>
@@ -2778,34 +2838,30 @@
         <v>&lt;attribute column='habitat' uri='http://purl.obolibrary.org/obo/ENVO_00002036' /&gt;</v>
       </c>
       <c r="H15" s="27" t="s">
-        <v>203</v>
+        <v>296</v>
       </c>
       <c r="I15" s="45" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>141</v>
-      </c>
+      <c r="B16" s="13"/>
       <c r="C16" s="13" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='substratum' uri='http://purl.obolibrary.org/obo/ENVO_00010483' /&gt;</v>
-      </c>
+      <c r="E16" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="27" t="s">
-        <v>202</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="13" t="s">
@@ -2815,19 +2871,19 @@
         <v>141</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>14</v>
+        <v>294</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G17" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='samplingProtocol' uri='http://rs.tdwg.org/dwc/terms/samplingProtocol' /&gt;</v>
+        <v>&lt;attribute column='substratum' uri='http://purl.obolibrary.org/obo/ENVO_00010483' /&gt;</v>
       </c>
       <c r="H17" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2838,21 +2894,19 @@
         <v>141</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="13"/>
-      <c r="E18" s="13" t="s">
-        <v>234</v>
-      </c>
+      <c r="E18" s="13"/>
       <c r="F18" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='minimumDepthInMeters' uri='http://rs.tdwg.org/dwc/terms/minimumDepthInMeters' /&gt;</v>
+        <v>&lt;attribute column='samplingProtocol' uri='http://rs.tdwg.org/dwc/terms/samplingProtocol' /&gt;</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2863,38 +2917,47 @@
         <v>141</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G19" s="13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='maximumDepthInMeters' uri='http://rs.tdwg.org/dwc/terms/maximumDepthInMeters' /&gt;</v>
+        <v>&lt;attribute column='minimumDepthInMeters' uri='http://rs.tdwg.org/dwc/terms/minimumDepthInMeters' /&gt;</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B20" s="13"/>
+      <c r="B20" s="13" t="s">
+        <v>141</v>
+      </c>
       <c r="C20" s="13" t="s">
-        <v>231</v>
+        <v>16</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="27"/>
+        <v>233</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G20" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='maximumDepthInMeters' uri='http://rs.tdwg.org/dwc/terms/maximumDepthInMeters' /&gt;</v>
+      </c>
+      <c r="H20" s="27" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="13" t="s">
@@ -2902,15 +2965,15 @@
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="13" t="s">
-        <v>276</v>
+        <v>230</v>
       </c>
       <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="13" t="s">
+        <v>232</v>
+      </c>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="27" t="s">
-        <v>277</v>
-      </c>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="13" t="s">
@@ -2918,15 +2981,15 @@
       </c>
       <c r="B22" s="13"/>
       <c r="C22" s="13" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="E22" s="13" t="s">
-        <v>235</v>
-      </c>
+      <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="27"/>
+      <c r="H22" s="27" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="13" t="s">
@@ -2934,69 +2997,58 @@
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="13" t="s">
-        <v>49</v>
+        <v>231</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="G23" s="13" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='eventRemarks' uri='http://rs.tdwg.org/dwc/terms/eventRemarks' /&gt;</v>
-      </c>
-      <c r="H23" s="27" t="s">
-        <v>153</v>
-      </c>
+      <c r="E23" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="27"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>182</v>
-      </c>
+      <c r="B24" s="13"/>
       <c r="C24" s="13" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G24" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='eventRemarks' uri='http://rs.tdwg.org/dwc/terms/eventRemarks' /&gt;</v>
+      </c>
+      <c r="H24" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="G24" s="13" t="str">
-        <f>CONCATENATE("&lt;attribute column='",$C24,"' uri='",$F24,"' /&gt;")</f>
+      <c r="G25" s="13" t="str">
+        <f>CONCATENATE("&lt;attribute column='",$C25,"' uri='",$F25,"' /&gt;")</f>
         <v>&lt;attribute column='recordedBy' uri='http://rs.tdwg.org/dwc/terms/recordedBy' /&gt;</v>
       </c>
-      <c r="H24" s="27" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>302</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>156</v>
-      </c>
-      <c r="G25" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='decimalLatitude' uri='http://rs.tdwg.org/dwc/terms/decimalLatitude' /&gt;</v>
-      </c>
-      <c r="H25" s="29" t="s">
-        <v>157</v>
+      <c r="H25" s="27" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -3007,20 +3059,20 @@
         <v>155</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>242</v>
+        <v>295</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G26" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='decimalLongitude' uri='ttp://rs.tdwg.org/dwc/terms/decimalLongitude' /&gt;</v>
+        <v>&lt;attribute column='decimalLatitude' uri='http://rs.tdwg.org/dwc/terms/decimalLatitude' /&gt;</v>
       </c>
       <c r="H26" s="29" t="s">
         <v>157</v>
@@ -3034,67 +3086,73 @@
         <v>155</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G27" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='coordinateUncertaintyInMeters' uri='http://rs.tdwg.org/dwc/terms/coordinateUncertaintyInMeters' /&gt;</v>
+        <v>&lt;attribute column='decimalLongitude' uri='ttp://rs.tdwg.org/dwc/terms/decimalLongitude' /&gt;</v>
       </c>
       <c r="H27" s="29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="28">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="14"/>
+      <c r="B28" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="C28" s="28" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="G28" s="28"/>
+        <v>159</v>
+      </c>
+      <c r="G28" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='coordinateUncertaintyInMeters' uri='http://rs.tdwg.org/dwc/terms/coordinateUncertaintyInMeters' /&gt;</v>
+      </c>
       <c r="H28" s="29" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28">
       <c r="A29" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>155</v>
-      </c>
+      <c r="B29" s="14"/>
       <c r="C29" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+        <v>235</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>240</v>
+      </c>
       <c r="F29" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="G29" s="28" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='country' uri='http://rs.tdwg.org/dwc/terms/country' /&gt;</v>
-      </c>
-      <c r="H29" s="29"/>
+        <v>236</v>
+      </c>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="28" t="s">
@@ -3104,16 +3162,16 @@
         <v>155</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
       <c r="F30" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G30" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='stateProvince' uri='http://rs.tdwg.org/dwc/terms/stateProvince' /&gt;</v>
+        <v>&lt;attribute column='country' uri='http://rs.tdwg.org/dwc/terms/country' /&gt;</v>
       </c>
       <c r="H30" s="29"/>
     </row>
@@ -3121,18 +3179,20 @@
       <c r="A31" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="14"/>
+      <c r="B31" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="C31" s="28" t="s">
-        <v>241</v>
+        <v>21</v>
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28" t="s">
-        <v>240</v>
+        <v>162</v>
       </c>
       <c r="G31" s="28" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='island' uri='http://rs.tdwg.org/dwc/terms/island' /&gt;</v>
+        <v>&lt;attribute column='stateProvince' uri='http://rs.tdwg.org/dwc/terms/stateProvince' /&gt;</v>
       </c>
       <c r="H31" s="29"/>
     </row>
@@ -3142,92 +3202,88 @@
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="28" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28"/>
       <c r="F32" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="G32" s="28"/>
+        <v>238</v>
+      </c>
+      <c r="G32" s="28" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='island' uri='http://rs.tdwg.org/dwc/terms/island' /&gt;</v>
+      </c>
       <c r="H32" s="29"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="G33" s="28"/>
+      <c r="H33" s="29"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C34" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="F33" s="28" t="s">
+      <c r="D34" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="F34" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="G33" s="28" t="str">
+      <c r="G34" s="28" t="str">
         <f t="shared" si="0"/>
         <v>&lt;attribute column='locality' uri='http://rs.tdwg.org/dwc/terms/locality' /&gt;</v>
       </c>
-      <c r="H33" s="29" t="s">
+      <c r="H34" s="29" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="6" customFormat="1">
-      <c r="A34" s="47" t="s">
+    <row r="35" spans="1:9" s="6" customFormat="1">
+      <c r="A35" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="47" t="s">
+      <c r="B35" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="C34" s="47" t="s">
-        <v>245</v>
-      </c>
-      <c r="D34" s="47" t="s">
-        <v>215</v>
-      </c>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47" t="s">
+      <c r="C35" s="47" t="s">
+        <v>243</v>
+      </c>
+      <c r="D35" s="47" t="s">
+        <v>214</v>
+      </c>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="G34" s="47" t="str">
-        <f>CONCATENATE("&lt;attribute column='",$C34,"' uri='",$F34,"' /&gt;")</f>
+      <c r="G35" s="47" t="str">
+        <f>CONCATENATE("&lt;attribute column='",$C35,"' uri='",$F35,"' /&gt;")</f>
         <v>&lt;attribute column='basisOfIdentification' uri='urn:basisOfID' /&gt;</v>
       </c>
-      <c r="H34" s="53" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="28">
-      <c r="A35" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="G35" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='identifiedBy' uri='http://rs.tdwg.org/dwc/terms/identifiedBy' /&gt;</v>
-      </c>
-      <c r="H35" s="31" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="H35" s="53" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="28">
       <c r="A36" s="30" t="s">
         <v>165</v>
       </c>
@@ -3235,19 +3291,19 @@
         <v>166</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G36" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='yearIdentified' uri='urn:yearIdentified' /&gt;</v>
+        <v>&lt;attribute column='identifiedBy' uri='http://rs.tdwg.org/dwc/terms/identifiedBy' /&gt;</v>
       </c>
       <c r="H36" s="31" t="s">
-        <v>134</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -3258,19 +3314,19 @@
         <v>166</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G37" s="30" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='monthIdentified' uri='urn:monthIdentified' /&gt;</v>
+        <v>&lt;attribute column='yearIdentified' uri='urn:yearIdentified' /&gt;</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -3281,45 +3337,43 @@
         <v>166</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G38" s="30" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;attribute column='monthIdentified' uri='urn:monthIdentified' /&gt;</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="30" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="30" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;attribute column='dayIdentified' uri='urn:dayIdentified' /&gt;</v>
       </c>
-      <c r="H38" s="31" t="s">
+      <c r="H39" s="31" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" s="7" customFormat="1">
-      <c r="A39" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="B39" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>228</v>
-      </c>
-      <c r="E39" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="G39" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='genus' uri='http://rs.tdwg.org/dwc/terms/genus' /&gt;</v>
-      </c>
-      <c r="H39" s="33"/>
     </row>
     <row r="40" spans="1:9" s="7" customFormat="1">
       <c r="A40" s="32" t="s">
@@ -3329,60 +3383,61 @@
         <v>172</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F40" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G40" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='species' uri='http://rs.tdwg.org/dwc/terms/specificEpithet' /&gt;</v>
+        <v>&lt;attribute column='genus' uri='http://rs.tdwg.org/dwc/terms/genus' /&gt;</v>
       </c>
       <c r="H40" s="33"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" s="7" customFormat="1">
       <c r="A41" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B41" s="32"/>
+      <c r="B41" s="32" t="s">
+        <v>172</v>
+      </c>
       <c r="C41" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
+        <v>28</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="F41" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="G41" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='species' uri='http://rs.tdwg.org/dwc/terms/specificEpithet' /&gt;</v>
+      </c>
       <c r="H41" s="33"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B42" s="32" t="s">
-        <v>172</v>
-      </c>
+      <c r="B42" s="32"/>
       <c r="C42" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="G42" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='vernacularName' uri='http://rs.tdwg.org/dwc/terms/vernacularName' /&gt;</v>
-      </c>
-      <c r="H42" s="33" t="s">
-        <v>289</v>
-      </c>
-      <c r="I42" s="45"/>
+        <v>244</v>
+      </c>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="33"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="32" t="s">
@@ -3392,66 +3447,67 @@
         <v>172</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D43" s="17"/>
-      <c r="E43" s="17" t="s">
-        <v>290</v>
-      </c>
+      <c r="E43" s="17"/>
       <c r="F43" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G43" s="32" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;attribute column='vernacularName' uri='http://rs.tdwg.org/dwc/terms/vernacularName' /&gt;</v>
+      </c>
+      <c r="H43" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="I43" s="45"/>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="F44" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" s="32" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;attribute column='kingdom' uri='http://rs.tdwg.org/dwc/terms/kingdom' /&gt;</v>
       </c>
-      <c r="H43" s="33"/>
-    </row>
-    <row r="44" spans="1:9" s="6" customFormat="1">
-      <c r="A44" s="51" t="s">
+      <c r="H44" s="33"/>
+    </row>
+    <row r="45" spans="1:9" s="6" customFormat="1">
+      <c r="A45" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B45" s="51" t="s">
         <v>172</v>
       </c>
-      <c r="C44" s="16" t="s">
+      <c r="C45" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="16" t="s">
-        <v>215</v>
-      </c>
-      <c r="E44" s="16"/>
-      <c r="F44" s="51" t="s">
+      <c r="D45" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="E45" s="16"/>
+      <c r="F45" s="51" t="s">
         <v>177</v>
       </c>
-      <c r="G44" s="51" t="str">
+      <c r="G45" s="51" t="str">
         <f t="shared" si="0"/>
         <v>&lt;attribute column='phylum' uri='http://rs.tdwg.org/dwc/terms/phylum' /&gt;</v>
       </c>
-      <c r="H44" s="52"/>
-    </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="B45" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="F45" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="G45" s="32" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='class' uri='http://rs.tdwg.org/dwc/terms/class' /&gt;</v>
-      </c>
-      <c r="H45" s="33"/>
+      <c r="H45" s="52"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="32" t="s">
@@ -3461,18 +3517,18 @@
         <v>172</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="17" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F46" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G46" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='order' uri='http://rs.tdwg.org/dwc/terms/order' /&gt;</v>
+        <v>&lt;attribute column='class' uri='http://rs.tdwg.org/dwc/terms/class' /&gt;</v>
       </c>
       <c r="H46" s="33"/>
     </row>
@@ -3484,41 +3540,43 @@
         <v>172</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="F47" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="G47" s="34" t="str">
+        <v>286</v>
+      </c>
+      <c r="F47" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="G47" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='family' uri='http://rs.tdwg.org/dwc/terms/family' /&gt;</v>
-      </c>
-      <c r="H47" s="35"/>
+        <v>&lt;attribute column='order' uri='http://rs.tdwg.org/dwc/terms/order' /&gt;</v>
+      </c>
+      <c r="H47" s="33"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32" t="s">
-        <v>248</v>
-      </c>
-      <c r="D48" s="32"/>
+      <c r="B48" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" s="17"/>
       <c r="E48" s="17" t="s">
-        <v>290</v>
-      </c>
-      <c r="F48" s="32" t="s">
-        <v>247</v>
-      </c>
-      <c r="G48" s="32" t="str">
+        <v>286</v>
+      </c>
+      <c r="F48" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="G48" s="34" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='taxonRemarks' uri='http://rs.tdwg.org/dwc/terms/taxonRemarks' /&gt;</v>
-      </c>
-      <c r="H48" s="33"/>
+        <v>&lt;attribute column='family' uri='http://rs.tdwg.org/dwc/terms/family' /&gt;</v>
+      </c>
+      <c r="H48" s="35"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="32" t="s">
@@ -3526,19 +3584,20 @@
       </c>
       <c r="B49" s="32"/>
       <c r="C49" s="32" t="s">
-        <v>249</v>
-      </c>
-      <c r="D49" s="32" t="s">
-        <v>228</v>
-      </c>
-      <c r="E49" s="32" t="s">
-        <v>251</v>
-      </c>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="33" t="s">
-        <v>250</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="D49" s="32"/>
+      <c r="E49" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="F49" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="G49" s="32" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='taxonRemarks' uri='http://rs.tdwg.org/dwc/terms/taxonRemarks' /&gt;</v>
+      </c>
+      <c r="H49" s="33"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="32" t="s">
@@ -3546,39 +3605,36 @@
       </c>
       <c r="B50" s="32"/>
       <c r="C50" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="32" t="s">
-        <v>288</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="F50" s="32"/>
       <c r="G50" s="32"/>
       <c r="H50" s="33" t="s">
-        <v>278</v>
+        <v>248</v>
       </c>
     </row>
     <row r="51" spans="1:8">
-      <c r="A51" s="36" t="s">
-        <v>181</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="36" t="s">
-        <v>184</v>
-      </c>
-      <c r="G51" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='occurrenceID' uri='http://rs.tdwg.org/dwc/terms/occurrenceID' /&gt;</v>
-      </c>
-      <c r="H51" s="37" t="s">
-        <v>265</v>
+      <c r="A51" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="G51" s="32"/>
+      <c r="H51" s="33" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -3589,40 +3645,39 @@
         <v>182</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>253</v>
+        <v>36</v>
       </c>
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
-      <c r="F52" s="18" t="s">
-        <v>252</v>
+      <c r="F52" s="36" t="s">
+        <v>184</v>
       </c>
       <c r="G52" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='associatedMedia' uri='http://rs.tdwg.org/dwc/terms/associatedMedia' /&gt;</v>
+        <v>&lt;attribute column='occurrenceID' uri='http://rs.tdwg.org/dwc/terms/occurrenceID' /&gt;</v>
       </c>
       <c r="H52" s="37" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16">
       <c r="A53" s="36" t="s">
         <v>181</v>
       </c>
       <c r="B53" s="36"/>
       <c r="C53" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="D53" s="18"/>
+        <v>308</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>311</v>
+      </c>
       <c r="E53" s="18"/>
-      <c r="F53" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="G53" s="36" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='associatedReferences' uri='http://rs.tdwg.org/dwc/terms/associatedReferences' /&gt;</v>
-      </c>
+      <c r="F53" s="54" t="s">
+        <v>310</v>
+      </c>
+      <c r="G53" s="36"/>
       <c r="H53" s="37" t="s">
-        <v>274</v>
+        <v>309</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -3633,43 +3688,41 @@
         <v>182</v>
       </c>
       <c r="C54" s="18" t="s">
-        <v>38</v>
+        <v>251</v>
       </c>
       <c r="D54" s="18"/>
-      <c r="E54" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="F54" s="36" t="s">
-        <v>185</v>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18" t="s">
+        <v>250</v>
       </c>
       <c r="G54" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='preservative' uri='http://rs.tdwg.org/dwc/terms/preparations' /&gt;</v>
+        <v>&lt;attribute column='associatedMedia' uri='http://rs.tdwg.org/dwc/terms/associatedMedia' /&gt;</v>
       </c>
       <c r="H54" s="37" t="s">
-        <v>206</v>
+        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="B55" s="36" t="s">
-        <v>182</v>
-      </c>
+      <c r="B55" s="36"/>
       <c r="C55" s="18" t="s">
-        <v>39</v>
+        <v>269</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
-      <c r="F55" s="36" t="s">
-        <v>186</v>
+      <c r="F55" s="18" t="s">
+        <v>268</v>
       </c>
       <c r="G55" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='previousIdentifications' uri='http://rs.tdwg.org/dwc/terms/previousIdentifications' /&gt;</v>
-      </c>
-      <c r="H55" s="37"/>
+        <v>&lt;attribute column='associatedReferences' uri='http://rs.tdwg.org/dwc/terms/associatedReferences' /&gt;</v>
+      </c>
+      <c r="H55" s="37" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="36" t="s">
@@ -3679,18 +3732,22 @@
         <v>182</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
+      <c r="E56" s="18" t="s">
+        <v>253</v>
+      </c>
       <c r="F56" s="36" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G56" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='lifeStage' uri='http://rs.tdwg.org/dwc/terms/lifeStage' /&gt;</v>
-      </c>
-      <c r="H56" s="37"/>
+        <v>&lt;attribute column='preservative' uri='http://rs.tdwg.org/dwc/terms/preparations' /&gt;</v>
+      </c>
+      <c r="H56" s="37" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="36" t="s">
@@ -3700,22 +3757,18 @@
         <v>182</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D57" s="18"/>
-      <c r="E57" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="F57" s="38" t="s">
-        <v>188</v>
-      </c>
-      <c r="G57" s="38" t="str">
+      <c r="E57" s="18"/>
+      <c r="F57" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="G57" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='weight' uri=' http://purl.obolibrary.org/obo/PATO_0000128' /&gt;</v>
-      </c>
-      <c r="H57" s="37" t="s">
-        <v>257</v>
-      </c>
+        <v>&lt;attribute column='previousIdentifications' uri='http://rs.tdwg.org/dwc/terms/previousIdentifications' /&gt;</v>
+      </c>
+      <c r="H57" s="37"/>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="36" t="s">
@@ -3725,16 +3778,16 @@
         <v>182</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
-      <c r="F58" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="G58" s="38" t="str">
+      <c r="F58" s="36" t="s">
+        <v>187</v>
+      </c>
+      <c r="G58" s="36" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='weightUnit' uri='http://purl.obolibrary.org/obo/UO_0000002' /&gt;</v>
+        <v>&lt;attribute column='lifeStage' uri='http://rs.tdwg.org/dwc/terms/lifeStage' /&gt;</v>
       </c>
       <c r="H58" s="37"/>
     </row>
@@ -3746,21 +3799,21 @@
         <v>182</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F59" s="38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G59" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='length' uri='http://purl.obolibrary.org/obo/PATO_0000122' /&gt;</v>
+        <v>&lt;attribute column='weight' uri=' http://purl.obolibrary.org/obo/PATO_0000128' /&gt;</v>
       </c>
       <c r="H59" s="37" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -3771,16 +3824,16 @@
         <v>182</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
       <c r="F60" s="38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G60" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='lengthUnit' uri='http://purl.obolibrary.org/obo/UO_0000001' /&gt;</v>
+        <v>&lt;attribute column='weightUnit' uri='http://purl.obolibrary.org/obo/UO_0000002' /&gt;</v>
       </c>
       <c r="H60" s="37"/>
     </row>
@@ -3788,37 +3841,46 @@
       <c r="A61" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="B61" s="36"/>
+      <c r="B61" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="C61" s="18" t="s">
-        <v>269</v>
+        <v>43</v>
       </c>
       <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="18" t="s">
-        <v>268</v>
+      <c r="E61" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="F61" s="38" t="s">
+        <v>190</v>
       </c>
       <c r="G61" s="38" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;attribute column='sex' uri='http://rs.tdwg.org/dwc/terms/sex' /&gt;</v>
-      </c>
-      <c r="H61" s="37"/>
+        <v>&lt;attribute column='length' uri='http://purl.obolibrary.org/obo/PATO_0000122' /&gt;</v>
+      </c>
+      <c r="H61" s="37" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="B62" s="36"/>
+      <c r="B62" s="36" t="s">
+        <v>182</v>
+      </c>
       <c r="C62" s="18" t="s">
-        <v>280</v>
+        <v>44</v>
       </c>
       <c r="D62" s="18"/>
-      <c r="E62" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="F62" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="G62" s="38"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="G62" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='lengthUnit' uri='http://purl.obolibrary.org/obo/UO_0000001' /&gt;</v>
+      </c>
       <c r="H62" s="37"/>
     </row>
     <row r="63" spans="1:8">
@@ -3827,14 +3889,17 @@
       </c>
       <c r="B63" s="36"/>
       <c r="C63" s="18" t="s">
-        <v>46</v>
+        <v>265</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="G63" s="38"/>
+        <v>264</v>
+      </c>
+      <c r="G63" s="38" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='sex' uri='http://rs.tdwg.org/dwc/terms/sex' /&gt;</v>
+      </c>
       <c r="H63" s="37"/>
     </row>
     <row r="64" spans="1:8">
@@ -3843,230 +3908,302 @@
       </c>
       <c r="B64" s="36"/>
       <c r="C64" s="18" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
+      <c r="E64" s="18" t="s">
+        <v>278</v>
+      </c>
       <c r="F64" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="G64" s="38" t="str">
+        <v>277</v>
+      </c>
+      <c r="G64" s="38"/>
+      <c r="H64" s="37"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="36"/>
+      <c r="C65" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="G65" s="38"/>
+      <c r="H65" s="37"/>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="B66" s="36"/>
+      <c r="C66" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="D66" s="18"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="G66" s="38" t="str">
         <f t="shared" si="0"/>
         <v>&lt;attribute column='occurrenceRemarks' uri='http://rs.tdwg.org/dwc/terms/occurrenceRemarks' /&gt;</v>
       </c>
-      <c r="H64" s="37"/>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="B65" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="C65" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="20" t="s">
-        <v>194</v>
-      </c>
-      <c r="G65" s="20" t="str">
-        <f t="shared" si="0"/>
-        <v>&lt;attribute column='geneticTissueType' uri='urn:geneticTissueType' /&gt;</v>
-      </c>
-      <c r="H65" s="39" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="B66" s="19"/>
-      <c r="C66" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="D66" s="19"/>
-      <c r="E66" s="19"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-      <c r="H66" s="39" t="s">
-        <v>262</v>
-      </c>
+      <c r="H66" s="37"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="B67" s="19"/>
+      <c r="B67" s="19" t="s">
+        <v>193</v>
+      </c>
       <c r="C67" s="19" t="s">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="D67" s="19"/>
       <c r="E67" s="19"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-      <c r="H67" s="39"/>
+      <c r="F67" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="G67" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>&lt;attribute column='geneticTissueType' uri='urn:geneticTissueType' /&gt;</v>
+      </c>
+      <c r="H67" s="39" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="20" t="s">
-        <v>192</v>
-      </c>
+      <c r="A68" s="20"/>
       <c r="B68" s="19"/>
       <c r="C68" s="19" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D68" s="19"/>
       <c r="E68" s="19"/>
       <c r="F68" s="20"/>
       <c r="G68" s="20"/>
       <c r="H68" s="39" t="s">
-        <v>264</v>
+        <v>304</v>
       </c>
     </row>
     <row r="69" spans="1:8">
-      <c r="A69" s="20" t="s">
-        <v>192</v>
-      </c>
+      <c r="A69" s="20"/>
       <c r="B69" s="19"/>
       <c r="C69" s="19" t="s">
-        <v>261</v>
+        <v>303</v>
       </c>
       <c r="D69" s="19"/>
       <c r="E69" s="19"/>
       <c r="F69" s="20"/>
       <c r="G69" s="20"/>
-      <c r="H69" s="39"/>
+      <c r="H69" s="39" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70" s="19"/>
+      <c r="C70" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="39" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="71" spans="1:8">
-      <c r="A71" s="46" t="s">
-        <v>293</v>
+      <c r="A71" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="19"/>
+      <c r="C71" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="39" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:8">
-      <c r="A72" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B72" s="21" t="s">
+      <c r="A72" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="39" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="A74" s="46" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B75" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="C72" s="22" t="s">
+      <c r="C75" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="D72" s="22"/>
-      <c r="E72" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="F72" s="22" t="s">
+      <c r="D75" s="22"/>
+      <c r="E75" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="F75" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="G72" s="22" t="str">
+      <c r="G75" s="22" t="str">
         <f t="shared" si="0"/>
         <v>&lt;attribute column='nucleicAcidExtraction' uri='http://gensc.org/ns/mixs/nucleicAcidExtraction (see https://mixs-as-rdf.googlecode.com/svn/trunk/terms/index.htm#nucleicAcidExtraction)' /&gt;</v>
       </c>
-      <c r="H72" s="40" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B73" s="21"/>
-      <c r="C73" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="D73" s="22"/>
-      <c r="E73" s="22"/>
-      <c r="F73" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="G73" s="22"/>
-      <c r="H73" s="40"/>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B74" s="21" t="s">
+      <c r="H75" s="40" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B76" s="21"/>
+      <c r="C76" s="22" t="s">
+        <v>267</v>
+      </c>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="G76" s="22"/>
+      <c r="H76" s="40"/>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B77" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="C74" s="22" t="s">
+      <c r="C77" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="F74" s="22" t="s">
+      <c r="D77" s="22"/>
+      <c r="E77" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="F77" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="G74" s="22" t="str">
+      <c r="G77" s="22" t="str">
         <f t="shared" si="0"/>
         <v>&lt;attribute column='loci' uri='http://gensc.org/ns/mixs/targetGene (https://mixs-as-rdf.googlecode.com/svn/trunk/terms/index.htm#targetGene)' /&gt;</v>
       </c>
-      <c r="H74" s="40" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B75" s="22"/>
-      <c r="C75" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="F75" s="22"/>
-      <c r="G75" s="22"/>
-      <c r="H75" s="40" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B76" s="22"/>
-      <c r="C76" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76" s="22"/>
-      <c r="E76" s="22"/>
-      <c r="F76" s="22"/>
-      <c r="G76" s="22"/>
-      <c r="H76" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="C77" s="11" t="s">
-        <v>296</v>
-      </c>
-      <c r="H77" s="26" t="s">
-        <v>297</v>
+      <c r="H77" s="40" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="F78" s="22"/>
+      <c r="G78" s="22"/>
+      <c r="H78" s="40" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
+      <c r="A79" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="22"/>
+      <c r="G79" s="22"/>
+      <c r="H79" s="40" t="s">
         <v>283</v>
       </c>
-      <c r="C78" s="41" t="s">
-        <v>299</v>
-      </c>
-      <c r="D78" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="H78" s="42" t="s">
-        <v>298</v>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="H80" s="26" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C81" s="41" t="s">
+        <v>312</v>
+      </c>
+      <c r="D81" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="H81" s="42" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
+      <c r="A82" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C82" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="H82" s="42" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
+      <c r="C83" s="41" t="s">
+        <v>316</v>
+      </c>
+      <c r="E83" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="H83" s="42" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -4074,15 +4211,15 @@
     <hyperlink ref="F2" r:id="rId1"/>
     <hyperlink ref="F11" r:id="rId2" display="http://rs.tdwg.org/dwc/terms/month"/>
     <hyperlink ref="F5" r:id="rId3" display="http://rs.tdwg.org/dwc/terms/month"/>
-    <hyperlink ref="F16" r:id="rId4"/>
+    <hyperlink ref="F17" r:id="rId4"/>
     <hyperlink ref="F14" r:id="rId5"/>
     <hyperlink ref="F15" r:id="rId6"/>
-    <hyperlink ref="F47" r:id="rId7"/>
-    <hyperlink ref="F57" r:id="rId8"/>
-    <hyperlink ref="F58" r:id="rId9"/>
-    <hyperlink ref="F60" r:id="rId10"/>
-    <hyperlink ref="F59" r:id="rId11"/>
-    <hyperlink ref="F63" r:id="rId12"/>
+    <hyperlink ref="F48" r:id="rId7"/>
+    <hyperlink ref="F59" r:id="rId8"/>
+    <hyperlink ref="F60" r:id="rId9"/>
+    <hyperlink ref="F62" r:id="rId10"/>
+    <hyperlink ref="F61" r:id="rId11"/>
+    <hyperlink ref="F65" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4140,7 +4277,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I1" s="8" t="s">
         <v>7</v>
@@ -4295,7 +4432,7 @@
         <v>55</v>
       </c>
       <c r="H2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I2">
         <v>2009</v>
@@ -4464,7 +4601,7 @@
       <c r="AK7" s="44"/>
       <c r="AO7" s="5"/>
       <c r="AP7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:51">

</xml_diff>